<commit_message>
task list part 이름
</commit_message>
<xml_diff>
--- a/resources/works.xlsx
+++ b/resources/works.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ttkmw/beyond-eyesight/workasme/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BA8C408-575B-A04D-AD57-B9040E6F1C24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8680C9B0-0CC8-AE47-8CBC-57D051EBDBA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="540" windowWidth="28800" windowHeight="16040" activeTab="1" xr2:uid="{E31C5CC0-24F5-8942-ADB8-59899293243B}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1354" uniqueCount="519">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1371" uniqueCount="522">
   <si>
     <t>F</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2079,6 +2079,18 @@
   </si>
   <si>
     <t>조건부 렌더링</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>체인지업 오티</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4! 소스 찾기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소스찾기</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2546,8 +2558,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6F0613A8-F193-1746-9201-3E95CB31A162}" name="표3" displayName="표3" ref="A5:W95" totalsRowShown="0" dataDxfId="44">
-  <autoFilter ref="A5:W95" xr:uid="{F235149E-6CF9-B843-8E05-1F129098F0AD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6F0613A8-F193-1746-9201-3E95CB31A162}" name="표3" displayName="표3" ref="A5:W98" totalsRowShown="0" dataDxfId="44">
+  <autoFilter ref="A5:W98" xr:uid="{F235149E-6CF9-B843-8E05-1F129098F0AD}"/>
   <tableColumns count="23">
     <tableColumn id="1" xr3:uid="{2FEBF9ED-D1F3-CE44-B1BE-684C1DD3520D}" name="Start Date" dataDxfId="43"/>
     <tableColumn id="5" xr3:uid="{FFB9D5D7-A599-E345-B389-F7191FE29828}" name="Start Time" dataDxfId="42"/>
@@ -4175,10 +4187,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18853549-B466-0346-BACD-864EAEBAA247}">
-  <dimension ref="A3:W95"/>
+  <dimension ref="A3:W98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="125" zoomScaleNormal="223" workbookViewId="0">
-      <selection activeCell="G96" sqref="G96"/>
+    <sheetView tabSelected="1" topLeftCell="H86" zoomScale="125" zoomScaleNormal="223" workbookViewId="0">
+      <selection activeCell="J99" sqref="J99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -8711,7 +8723,9 @@
       <c r="C95" s="4">
         <v>44382</v>
       </c>
-      <c r="D95" s="2"/>
+      <c r="D95" s="10">
+        <v>0.875</v>
+      </c>
       <c r="E95" s="10" t="s">
         <v>164</v>
       </c>
@@ -8721,10 +8735,18 @@
       <c r="G95" s="2" t="s">
         <v>518</v>
       </c>
-      <c r="H95" s="2"/>
-      <c r="I95" s="2"/>
-      <c r="J95" s="2"/>
-      <c r="K95" s="2"/>
+      <c r="H95" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="I95" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="J95" s="2" t="s">
+        <v>518</v>
+      </c>
+      <c r="K95" s="2" t="s">
+        <v>512</v>
+      </c>
       <c r="L95" s="2"/>
       <c r="M95" s="2"/>
       <c r="N95" s="2"/>
@@ -8737,6 +8759,131 @@
       <c r="U95" s="2"/>
       <c r="V95" s="2"/>
       <c r="W95" s="2"/>
+    </row>
+    <row r="96" spans="1:23" ht="19">
+      <c r="A96" s="4">
+        <v>44382</v>
+      </c>
+      <c r="B96" s="10">
+        <v>0.875</v>
+      </c>
+      <c r="C96" s="4">
+        <v>44382</v>
+      </c>
+      <c r="D96" s="10">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="E96" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="F96" s="10" t="s">
+        <v>365</v>
+      </c>
+      <c r="G96" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="H96" s="2"/>
+      <c r="I96" s="2"/>
+      <c r="J96" s="2"/>
+      <c r="K96" s="2"/>
+      <c r="L96" s="2"/>
+      <c r="M96" s="2"/>
+      <c r="N96" s="2"/>
+      <c r="O96" s="2"/>
+      <c r="P96" s="2"/>
+      <c r="Q96" s="2"/>
+      <c r="R96" s="2"/>
+      <c r="S96" s="2"/>
+      <c r="T96" s="2"/>
+      <c r="U96" s="2"/>
+      <c r="V96" s="2"/>
+      <c r="W96" s="2"/>
+    </row>
+    <row r="97" spans="1:23" ht="19">
+      <c r="A97" s="4">
+        <v>44382</v>
+      </c>
+      <c r="B97" s="10">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C97" s="4">
+        <v>44382</v>
+      </c>
+      <c r="D97" s="10">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="E97" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="F97" s="10" t="s">
+        <v>365</v>
+      </c>
+      <c r="G97" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H97" s="2"/>
+      <c r="I97" s="2"/>
+      <c r="J97" s="2"/>
+      <c r="K97" s="2"/>
+      <c r="L97" s="2"/>
+      <c r="M97" s="2"/>
+      <c r="N97" s="2"/>
+      <c r="O97" s="2"/>
+      <c r="P97" s="2"/>
+      <c r="Q97" s="2"/>
+      <c r="R97" s="2"/>
+      <c r="S97" s="2"/>
+      <c r="T97" s="2"/>
+      <c r="U97" s="2"/>
+      <c r="V97" s="2"/>
+      <c r="W97" s="2"/>
+    </row>
+    <row r="98" spans="1:23" ht="19">
+      <c r="A98" s="4">
+        <v>44382</v>
+      </c>
+      <c r="B98" s="10">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="C98" s="4">
+        <v>44382</v>
+      </c>
+      <c r="D98" s="10">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="E98" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="F98" s="10" t="s">
+        <v>331</v>
+      </c>
+      <c r="G98" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="H98" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="I98" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="J98" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="K98" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="L98" s="2"/>
+      <c r="M98" s="2"/>
+      <c r="N98" s="2"/>
+      <c r="O98" s="2"/>
+      <c r="P98" s="2"/>
+      <c r="Q98" s="2"/>
+      <c r="R98" s="2"/>
+      <c r="S98" s="2"/>
+      <c r="T98" s="2"/>
+      <c r="U98" s="2"/>
+      <c r="V98" s="2"/>
+      <c r="W98" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>